<commit_message>
final results of alpha=2.5
</commit_message>
<xml_diff>
--- a/Homework 2/resultsV2.xlsx
+++ b/Homework 2/resultsV2.xlsx
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="C2" t="n">
-        <v>1.174069881439209</v>
+        <v>5.306968212127686</v>
       </c>
     </row>
     <row r="3">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>426</v>
+        <v>390</v>
       </c>
       <c r="C3" t="n">
-        <v>1.570884227752686</v>
+        <v>7.739184379577637</v>
       </c>
     </row>
     <row r="4">
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="C4" t="n">
-        <v>1.134962558746338</v>
+        <v>5.619730710983276</v>
       </c>
     </row>
     <row r="5">
@@ -488,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7996671199798584</v>
+        <v>4.020173311233521</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +499,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>482</v>
+        <v>404</v>
       </c>
       <c r="C6" t="n">
-        <v>1.410490751266479</v>
+        <v>7.428812503814697</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +510,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>337</v>
+        <v>296</v>
       </c>
       <c r="C7" t="n">
-        <v>1.049870729446411</v>
+        <v>6.137551546096802</v>
       </c>
     </row>
     <row r="8">
@@ -521,10 +521,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="C8" t="n">
-        <v>1.18963623046875</v>
+        <v>7.76811957359314</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C9" t="n">
-        <v>3.756444215774536</v>
+        <v>21.91056942939758</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>353</v>
+        <v>379</v>
       </c>
       <c r="C10" t="n">
-        <v>4.513932228088379</v>
+        <v>28.65278673171997</v>
       </c>
     </row>
     <row r="11">
@@ -554,10 +554,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>326</v>
+        <v>296</v>
       </c>
       <c r="C11" t="n">
-        <v>1.033243656158447</v>
+        <v>7.16151762008667</v>
       </c>
     </row>
     <row r="12">
@@ -565,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>526</v>
+        <v>480</v>
       </c>
       <c r="C12" t="n">
-        <v>2.086487293243408</v>
+        <v>14.11760377883911</v>
       </c>
     </row>
     <row r="13">
@@ -576,10 +576,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>465</v>
+        <v>406</v>
       </c>
       <c r="C13" t="n">
-        <v>1.72458815574646</v>
+        <v>10.33298563957214</v>
       </c>
     </row>
     <row r="14">
@@ -587,10 +587,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>694</v>
+        <v>685</v>
       </c>
       <c r="C14" t="n">
-        <v>1.65571141242981</v>
+        <v>12.52477717399597</v>
       </c>
     </row>
     <row r="15">
@@ -598,10 +598,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9317202568054199</v>
+        <v>6.341109752655029</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>113</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6616361141204834</v>
+        <v>4.343533277511597</v>
       </c>
     </row>
     <row r="17">
@@ -620,10 +620,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C17" t="n">
-        <v>1.429350137710571</v>
+        <v>8.937321424484253</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>169</v>
       </c>
       <c r="C18" t="n">
-        <v>1.208371162414551</v>
+        <v>10.12352561950684</v>
       </c>
     </row>
     <row r="19">
@@ -642,10 +642,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C19" t="n">
-        <v>1.670809268951416</v>
+        <v>10.86786365509033</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2896811962127686</v>
+        <v>1.777767896652222</v>
       </c>
     </row>
     <row r="21">
@@ -664,10 +664,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C21" t="n">
-        <v>0.909590482711792</v>
+        <v>6.24271035194397</v>
       </c>
     </row>
     <row r="22">
@@ -675,10 +675,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C22" t="n">
-        <v>1.878539562225342</v>
+        <v>14.68635034561157</v>
       </c>
     </row>
     <row r="23">
@@ -686,10 +686,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="C23" t="n">
-        <v>3.350117444992065</v>
+        <v>25.20130062103271</v>
       </c>
     </row>
     <row r="24">
@@ -697,10 +697,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C24" t="n">
-        <v>5.379126071929932</v>
+        <v>34.20357608795166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>